<commit_message>
fix clothing / add category hierarchy
</commit_message>
<xml_diff>
--- a/src/assets/ec-product-db/ec-product-table.xlsx
+++ b/src/assets/ec-product-db/ec-product-table.xlsx
@@ -526,22 +526,22 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>商品(衣類 / clothes)</t>
-    <rPh sb="0" eb="2">
-      <t>ショウヒン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>イルイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>商品(食品 / foods)</t>
     <rPh sb="0" eb="2">
       <t>ショウヒン</t>
     </rPh>
     <rPh sb="3" eb="5">
       <t>ショクヒン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>商品(衣類 / clothings)</t>
+    <rPh sb="0" eb="2">
+      <t>ショウヒン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>イルイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -870,19 +870,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -894,15 +887,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2148,142 +2148,148 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" ht="19">
-      <c r="I19" s="27" t="s">
+      <c r="I19" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="28"/>
+      <c r="J19" s="36"/>
       <c r="K19" s="9" t="s">
         <v>24</v>
       </c>
       <c r="L19" s="14"/>
     </row>
     <row r="20" spans="1:12" ht="19">
-      <c r="I20" s="25">
+      <c r="I20" s="32">
         <v>301</v>
       </c>
-      <c r="J20" s="29"/>
+      <c r="J20" s="37"/>
       <c r="K20" s="10">
         <v>10</v>
       </c>
       <c r="L20" s="15"/>
     </row>
     <row r="21" spans="1:12" ht="19">
-      <c r="I21" s="25">
+      <c r="I21" s="32">
         <v>301</v>
       </c>
-      <c r="J21" s="29"/>
+      <c r="J21" s="37"/>
       <c r="K21" s="10">
         <v>21</v>
       </c>
       <c r="L21" s="15"/>
     </row>
     <row r="22" spans="1:12" ht="19">
-      <c r="I22" s="25">
+      <c r="I22" s="32">
         <v>302</v>
       </c>
-      <c r="J22" s="29"/>
+      <c r="J22" s="37"/>
       <c r="K22" s="10">
         <v>11</v>
       </c>
       <c r="L22" s="15"/>
     </row>
     <row r="23" spans="1:12" ht="19">
-      <c r="I23" s="25">
+      <c r="I23" s="32">
         <v>302</v>
       </c>
-      <c r="J23" s="26"/>
+      <c r="J23" s="33"/>
       <c r="K23" s="10">
         <v>21</v>
       </c>
       <c r="L23" s="15"/>
     </row>
     <row r="24" spans="1:12" ht="19">
-      <c r="I24" s="25">
+      <c r="I24" s="32">
         <v>303</v>
       </c>
-      <c r="J24" s="26"/>
+      <c r="J24" s="33"/>
       <c r="K24" s="10">
         <v>12</v>
       </c>
       <c r="L24" s="15"/>
     </row>
     <row r="25" spans="1:12" ht="19">
-      <c r="I25" s="25">
+      <c r="I25" s="32">
         <v>303</v>
       </c>
-      <c r="J25" s="26"/>
+      <c r="J25" s="33"/>
       <c r="K25" s="10">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="19">
-      <c r="I26" s="25">
+      <c r="I26" s="32">
         <v>304</v>
       </c>
-      <c r="J26" s="26"/>
+      <c r="J26" s="33"/>
       <c r="K26" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="19">
-      <c r="I27" s="25">
+      <c r="I27" s="32">
         <v>304</v>
       </c>
-      <c r="J27" s="26"/>
+      <c r="J27" s="33"/>
       <c r="K27" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="19">
-      <c r="I28" s="25">
+      <c r="I28" s="32">
         <v>305</v>
       </c>
-      <c r="J28" s="26"/>
+      <c r="J28" s="33"/>
       <c r="K28" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="19">
-      <c r="I29" s="25">
+      <c r="I29" s="32">
         <v>305</v>
       </c>
-      <c r="J29" s="26"/>
+      <c r="J29" s="33"/>
       <c r="K29" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="19">
-      <c r="I30" s="31">
+      <c r="I30" s="30">
         <v>306</v>
       </c>
-      <c r="J30" s="33"/>
+      <c r="J30" s="34"/>
       <c r="K30" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="19">
-      <c r="I31" s="30">
+      <c r="I31" s="29">
         <v>306</v>
       </c>
-      <c r="J31" s="31"/>
+      <c r="J31" s="30"/>
       <c r="K31" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="19">
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
       <c r="K32" s="16"/>
       <c r="L32" s="16"/>
     </row>
     <row r="33" spans="9:12" ht="19">
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="I32:J32"/>
     <mergeCell ref="I33:J33"/>
@@ -2293,12 +2299,6 @@
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2847,8 +2847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:I45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2862,7 +2862,7 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:9" ht="22">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="25" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2930,13 +2930,13 @@
       <c r="F10" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="37" t="s">
+      <c r="I10" s="28" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2951,10 +2951,10 @@
       <c r="D11" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="28" t="s">
         <v>78</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -2972,8 +2972,8 @@
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
@@ -2983,21 +2983,21 @@
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="22">
       <c r="A14" s="1"/>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="25" t="s">
         <v>84</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
@@ -3007,8 +3007,8 @@
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
@@ -3016,12 +3016,12 @@
     <row r="16" spans="1:9" ht="19">
       <c r="A16" s="1"/>
       <c r="B16" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
@@ -3031,8 +3031,8 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
@@ -3076,20 +3076,20 @@
     <row r="21" spans="1:9" ht="19">
       <c r="A21" s="1"/>
       <c r="B21" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:9" ht="19">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" spans="1:9" ht="19">
       <c r="A23" s="1"/>
@@ -3146,7 +3146,7 @@
     </row>
     <row r="28" spans="1:9" ht="22">
       <c r="A28" s="1"/>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="26" t="s">
         <v>83</v>
       </c>
       <c r="C28" s="1"/>
@@ -3198,19 +3198,19 @@
     </row>
     <row r="37" spans="2:6" ht="19">
       <c r="B37" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
     </row>
     <row r="38" spans="2:6" ht="19">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
     </row>
     <row r="39" spans="2:6" ht="19">
       <c r="B39" s="12" t="s">
@@ -3247,19 +3247,19 @@
     </row>
     <row r="42" spans="2:6" ht="19">
       <c r="B42" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
     </row>
     <row r="43" spans="2:6" ht="19">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
     </row>
     <row r="44" spans="2:6" ht="19">
       <c r="B44" s="12" t="s">

</xml_diff>